<commit_message>
Added rendered pictures, excel and made a check for stack overflow
</commit_message>
<xml_diff>
--- a/final-project-workload.xlsx
+++ b/final-project-workload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eexua\Documents\1.CSE\Year_4\CG\Assignments\final_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eexua\Documents\1.CSE\Year_4\CG\Assignments\cg-group-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91A19330-DC96-4C07-82E4-13905A208FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB3DD52-9CB9-4269-977F-46247C385FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="885" yWindow="585" windowWidth="28770" windowHeight="17100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workload" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Fill in the percentages with values in range [0-100]</t>
   </si>
@@ -85,42 +85,6 @@
   </si>
   <si>
     <t>texture mapping</t>
-  </si>
-  <si>
-    <t>extra features</t>
-  </si>
-  <si>
-    <t>Environment maps.</t>
-  </si>
-  <si>
-    <t>SAH+binning as splitting criterion for BVH</t>
-  </si>
-  <si>
-    <t>Motion blur</t>
-  </si>
-  <si>
-    <t>Bloom filter on the final image</t>
-  </si>
-  <si>
-    <t>Texture filtering: Bilinear interpolation</t>
-  </si>
-  <si>
-    <t>Texture filtering: Mipmapping</t>
-  </si>
-  <si>
-    <t>Cast multiple rays per pixel with irregular sampling</t>
-  </si>
-  <si>
-    <t>Glossy reflections</t>
-  </si>
-  <si>
-    <t>Transparency</t>
-  </si>
-  <si>
-    <t>Depth of field</t>
-  </si>
-  <si>
-    <t>total (basic + extra)</t>
   </si>
   <si>
     <t>TVJuCSlpMECM04q0LeCIezuP1cwF6_FBoiqTNqy2CiBUMTNJR0JBTDFWUEc1NDBCRDhWTk01RDhYOSQlQCN0PWcu</t>
@@ -216,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -252,74 +216,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,27 +272,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -781,46 +661,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="3" width="48.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="10.54296875" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -834,35 +715,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="4">
-        <v>1</v>
+        <v>5228093</v>
       </c>
       <c r="E5" s="4">
-        <v>2</v>
+        <v>4907531</v>
       </c>
       <c r="F5" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>4917456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -877,7 +758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
@@ -894,11 +775,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" ref="G8:G15" si="0">SUM(D8:F8)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
@@ -915,11 +795,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>9</v>
       </c>
@@ -936,11 +815,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>10</v>
       </c>
@@ -957,11 +835,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>11</v>
       </c>
@@ -978,11 +855,10 @@
         <v>100</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
         <v>12</v>
       </c>
@@ -999,11 +875,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>13</v>
       </c>
@@ -1020,11 +895,10 @@
         <v>100</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>14</v>
       </c>
@@ -1041,303 +915,116 @@
         <v>0</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="19">
-        <f>SUM(C8:C15)</f>
         <v>18</v>
       </c>
       <c r="D16" s="20">
-        <f>SUMPRODUCT(C8:C15,D8:D15)/100</f>
         <v>6.01</v>
       </c>
       <c r="E16" s="20">
-        <f>SUMPRODUCT($C8:$C15,E8:E15)/100</f>
         <v>5.99</v>
       </c>
       <c r="F16" s="20">
-        <f>SUMPRODUCT($C8:$C15,F8:F15)/100</f>
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
-      <c r="B18" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B18"/>
+      <c r="C18"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
-      <c r="B19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="D19" s="23">
-        <v>100</v>
-      </c>
-      <c r="E19" s="11">
-        <v>0</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0</v>
-      </c>
-      <c r="G19" s="6">
-        <f t="shared" ref="G19:G28" si="1">SUM(D19:F19)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="D20" s="23">
-        <v>0</v>
-      </c>
-      <c r="E20" s="11">
-        <v>0</v>
-      </c>
-      <c r="F20" s="12">
-        <v>0</v>
-      </c>
-      <c r="G20" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="22">
-        <v>2.5</v>
-      </c>
-      <c r="D21" s="23">
-        <v>0</v>
-      </c>
-      <c r="E21" s="11">
-        <v>0</v>
-      </c>
-      <c r="F21" s="12">
-        <v>100</v>
-      </c>
-      <c r="G21" s="6">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="D22" s="23">
-        <v>0</v>
-      </c>
-      <c r="E22" s="11">
-        <v>0</v>
-      </c>
-      <c r="F22" s="12">
-        <v>100</v>
-      </c>
-      <c r="G22" s="6">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="D23" s="23">
-        <v>100</v>
-      </c>
-      <c r="E23" s="11">
-        <v>0</v>
-      </c>
-      <c r="F23" s="12">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="22">
-        <v>2</v>
-      </c>
-      <c r="D24" s="23">
-        <v>100</v>
-      </c>
-      <c r="E24" s="11">
-        <v>0</v>
-      </c>
-      <c r="F24" s="12">
-        <v>0</v>
-      </c>
-      <c r="G24" s="6">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="D25" s="23">
-        <v>0</v>
-      </c>
-      <c r="E25" s="11">
-        <v>0</v>
-      </c>
-      <c r="F25" s="12">
-        <v>0</v>
-      </c>
-      <c r="G25" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="22">
-        <v>2.5</v>
-      </c>
-      <c r="D26" s="23">
-        <v>0</v>
-      </c>
-      <c r="E26" s="11">
-        <v>100</v>
-      </c>
-      <c r="F26" s="12">
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="D27" s="23">
-        <v>0</v>
-      </c>
-      <c r="E27" s="11">
-        <v>100</v>
-      </c>
-      <c r="F27" s="12">
-        <v>0</v>
-      </c>
-      <c r="G27" s="6">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="22">
-        <v>3</v>
-      </c>
-      <c r="D28" s="23">
-        <v>0</v>
-      </c>
-      <c r="E28" s="11">
-        <v>0</v>
-      </c>
-      <c r="F28" s="12">
-        <v>0</v>
-      </c>
-      <c r="G28" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="25">
-        <f>SUM(C19:C28)</f>
-        <v>18</v>
-      </c>
-      <c r="D29" s="20">
-        <f>SUMPRODUCT($C19:$C28,D19:D28)/100</f>
-        <v>4</v>
-      </c>
-      <c r="E29" s="20">
-        <f>SUMPRODUCT($C19:$C28,E19:E28)/100</f>
-        <v>4</v>
-      </c>
-      <c r="F29" s="20">
-        <f>SUMPRODUCT($C19:$C28,F19:F28)/100</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="28">
-        <f>D$16+D29</f>
-        <v>10.01</v>
-      </c>
-      <c r="E31" s="28">
-        <f>E$16+E29</f>
-        <v>9.99</v>
-      </c>
-      <c r="F31" s="29">
-        <f>F$16+F29</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B19"/>
+      <c r="C19"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+      <c r="C20"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+      <c r="C21"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+      <c r="C22"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="C23"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25"/>
+      <c r="C25"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+      <c r="C26"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27"/>
+      <c r="C27"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+      <c r="C30"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+      <c r="C31"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32"/>
+      <c r="C32"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+      <c r="C33"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34"/>
+      <c r="C34"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35"/>
+      <c r="C35"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36"/>
+      <c r="C36"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+      <c r="C37"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38"/>
+      <c r="C38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1355,21 +1042,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30" t="s">
-        <v>29</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>